<commit_message>
Finish XLX to JSON + Manogo
</commit_message>
<xml_diff>
--- a/stuff/National-Minimum-Wage.xlsx
+++ b/stuff/National-Minimum-Wage.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="427">
   <si>
     <t xml:space="preserve">COUNTRY</t>
   </si>
@@ -34,18 +34,12 @@
     <t xml:space="preserve">Dollars</t>
   </si>
   <si>
-    <t xml:space="preserve">https://countryeconomy.com/national-minimum-wage</t>
-  </si>
-  <si>
     <t xml:space="preserve">United States </t>
   </si>
   <si>
     <t xml:space="preserve">1,256.7</t>
   </si>
   <si>
-    <t xml:space="preserve">1,256.7 </t>
-  </si>
-  <si>
     <t xml:space="preserve">United Kingdom </t>
   </si>
   <si>
@@ -133,6 +127,9 @@
     <t xml:space="preserve">5,000.0</t>
   </si>
   <si>
+    <t xml:space="preserve">67.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">Albania </t>
   </si>
   <si>
@@ -334,6 +331,9 @@
     <t xml:space="preserve">60,000.0</t>
   </si>
   <si>
+    <t xml:space="preserve">100.53</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chile </t>
   </si>
   <si>
@@ -472,9 +472,15 @@
     <t xml:space="preserve">150,000.0</t>
   </si>
   <si>
+    <t xml:space="preserve">251.32</t>
+  </si>
+  <si>
     <t xml:space="preserve">Georgia </t>
   </si>
   <si>
+    <t xml:space="preserve">350.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">117.85 </t>
   </si>
   <si>
@@ -529,6 +535,9 @@
     <t xml:space="preserve">35,000.0</t>
   </si>
   <si>
+    <t xml:space="preserve">168.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hong Kong </t>
   </si>
   <si>
@@ -562,6 +571,9 @@
     <t xml:space="preserve">6,500.0</t>
   </si>
   <si>
+    <t xml:space="preserve">68.04</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hungary </t>
   </si>
   <si>
@@ -649,6 +661,9 @@
     <t xml:space="preserve">80.0</t>
   </si>
   <si>
+    <t xml:space="preserve">180.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">Comoros </t>
   </si>
   <si>
@@ -754,6 +769,9 @@
     <t xml:space="preserve">450.0</t>
   </si>
   <si>
+    <t xml:space="preserve">320.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">Morocco </t>
   </si>
   <si>
@@ -1051,6 +1069,9 @@
     <t xml:space="preserve">2,167.0</t>
   </si>
   <si>
+    <t xml:space="preserve">22.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">Saudi Arabia </t>
   </si>
   <si>
@@ -1069,6 +1090,9 @@
     <t xml:space="preserve">425.0</t>
   </si>
   <si>
+    <t xml:space="preserve">70.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">Slovenia </t>
   </si>
   <si>
@@ -1091,6 +1115,9 @@
   </si>
   <si>
     <t xml:space="preserve">25,000.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57.00</t>
   </si>
   <si>
     <t xml:space="preserve">Senegal </t>
@@ -1384,12 +1411,12 @@
   <dimension ref="A1:E146"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E83" activeCellId="0" sqref="E83"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="61.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
@@ -1410,481 +1437,479 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>2013</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>67</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C13" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>2014</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C15" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C17" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C19" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C20" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C21" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C22" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="C23" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>2013</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="0" t="n">
-        <v>2013</v>
-      </c>
-      <c r="C25" s="0" t="s">
+      <c r="D25" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="C26" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C27" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C28" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>82</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C29" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="0" t="n">
-        <v>2013</v>
-      </c>
-      <c r="C29" s="0" t="s">
+      <c r="D29" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="0" t="n">
-        <v>2013</v>
-      </c>
-      <c r="C30" s="0" t="s">
+      <c r="D30" s="0" t="s">
         <v>88</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C31" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>2012</v>
       </c>
       <c r="C32" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C33" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="C34" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C35" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="D35" s="0" t="n">
-        <v>100535</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2063,7 +2088,7 @@
         <v>2013</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>141</v>
@@ -2107,699 +2132,699 @@
       <c r="C51" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="D51" s="0" t="n">
-        <v>251327</v>
+      <c r="D51" s="0" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>2018</v>
       </c>
-      <c r="C52" s="0" t="n">
-        <v>350</v>
+      <c r="C52" s="0" t="s">
+        <v>152</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="D58" s="0" t="n">
-        <v>168.1</v>
+        <v>170</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="D62" s="0" t="n">
-        <v>68.04</v>
+        <v>182</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>2012</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="D72" s="0" t="n">
-        <v>180</v>
+        <v>212</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>2009</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="D84" s="0" t="n">
-        <v>320</v>
+        <v>248</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>2016</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>2010</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>2013</v>
@@ -2808,643 +2833,640 @@
         <v>132</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="B103" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="B104" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="B105" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="B106" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="B107" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="B108" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="B109" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="B110" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="B111" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="B112" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="B113" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="B114" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="B115" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="B116" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="B117" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="B118" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>342</v>
-      </c>
-      <c r="D118" s="0" t="n">
-        <v>22</v>
+        <v>348</v>
+      </c>
+      <c r="D118" s="0" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="B119" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="B120" s="0" t="n">
         <v>2010</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="B121" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="D121" s="0" t="n">
-        <v>70</v>
+        <v>355</v>
+      </c>
+      <c r="D121" s="0" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="B122" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="B123" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="B124" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="D124" s="0" t="n">
-        <v>57</v>
+        <v>364</v>
+      </c>
+      <c r="D124" s="0" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="B125" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="B126" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="B127" s="0" t="n">
         <v>2010</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="B128" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="B129" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="B130" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="B131" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="B132" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="B133" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="B134" s="0" t="n">
         <v>2012</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="B135" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="B136" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="D136" s="0" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="B137" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="D137" s="0" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="B138" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="D138" s="0" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
       <c r="B139" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="D139" s="0" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="B140" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="D140" s="0" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="B141" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="D141" s="0" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
       <c r="B142" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="D142" s="0" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="B143" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
       <c r="D143" s="0" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
       <c r="B144" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
       <c r="D144" s="0" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="B145" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="D145" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="B146" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D146" s="0" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E1" r:id="rId1" display="https://countryeconomy.com/national-minimum-wage"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>